<commit_message>
Updated Box Office by Country and Google Maps notebook
</commit_message>
<xml_diff>
--- a/Datasets/Box_Office_by_Country.xlsx
+++ b/Datasets/Box_Office_by_Country.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee Wealth Mgmt\Documents\GitHub\Group-Project-One_UDENDATA\Datasets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee Wealth Mgmt\Documents\GitHub\Team-Aurora-Marvels\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81F6233-E3F1-43DB-BD9E-0F0CA412A137}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53468562-86DD-4367-812A-6A0A04FFD248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" xr2:uid="{52C63866-7CA8-46D1-AE34-6D66B8611C4C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="63">
   <si>
     <t>Country</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Portugal</t>
   </si>
   <si>
-    <t>Russia (CIS)</t>
-  </si>
-  <si>
     <t>Slovakia</t>
   </si>
   <si>
@@ -219,6 +216,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>Russia</t>
   </si>
 </sst>
 </file>
@@ -595,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5B63F0-7E42-422D-B61C-0353DBECD408}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V22" sqref="V22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,97 +638,97 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>3357295</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="1">
         <v>4126139</v>
@@ -757,16 +757,16 @@
         <v>5720345</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K2" s="1">
         <v>4318696</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M2" s="1">
         <v>28673092</v>
@@ -781,19 +781,19 @@
         <v>3460732</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V2" s="1">
         <v>3852313</v>
@@ -802,19 +802,19 @@
         <v>5148269</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z2" s="1">
         <v>7033029</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC2" s="1">
         <v>5475083</v>
@@ -826,7 +826,7 @@
         <v>2830282</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>8654635</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E3" s="1">
         <v>11681785</v>
@@ -855,37 +855,37 @@
         <v>31932114</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K3" s="1">
         <v>24755435</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M3" s="1">
         <v>44722076</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="P3" s="1">
         <v>15902123</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W3" s="1">
         <v>17295477</v>
@@ -894,13 +894,13 @@
         <v>21880008</v>
       </c>
       <c r="Y3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z3" s="1">
         <v>20264403</v>
       </c>
       <c r="AA3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC3" s="1">
         <v>21446060</v>
@@ -912,7 +912,7 @@
         <v>15667184</v>
       </c>
       <c r="AF3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
@@ -941,7 +941,7 @@
         <v>36942424</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J4" s="1">
         <v>28317546</v>
@@ -950,7 +950,7 @@
         <v>30563398</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M4" s="1">
         <v>27066360</v>
@@ -968,16 +968,16 @@
         <v>14485312</v>
       </c>
       <c r="R4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V4" s="1">
         <v>11694313</v>
@@ -986,16 +986,16 @@
         <v>29218096</v>
       </c>
       <c r="X4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z4" s="1">
         <v>31896084</v>
       </c>
       <c r="AA4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB4" s="1">
         <v>12092872</v>
@@ -1010,7 +1010,7 @@
         <v>19031136</v>
       </c>
       <c r="AF4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.25">
@@ -1021,7 +1021,7 @@
         <v>310618</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D5" s="1">
         <v>385465</v>
@@ -1039,16 +1039,16 @@
         <v>636460</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K5" s="1">
         <v>474412</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M5" s="1">
         <v>482445</v>
@@ -1063,31 +1063,31 @@
         <v>557862</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W5" s="1">
         <v>295183</v>
       </c>
       <c r="X5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z5" s="1">
         <v>328580</v>
@@ -1096,7 +1096,7 @@
         <v>379034</v>
       </c>
       <c r="AB5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC5" s="1">
         <v>879675</v>
@@ -1108,7 +1108,7 @@
         <v>859396</v>
       </c>
       <c r="AF5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.25">
@@ -1119,10 +1119,10 @@
         <v>89100000</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E6" s="1">
         <v>105718824</v>
@@ -1137,22 +1137,22 @@
         <v>104600000</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K6" s="1">
         <v>153110000</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O6" s="1">
         <v>42453208</v>
@@ -1161,43 +1161,43 @@
         <v>110300000</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W6" s="1">
         <v>105962992</v>
       </c>
       <c r="X6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z6" s="1">
         <v>118888328</v>
       </c>
       <c r="AA6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD6" s="1">
         <v>112000000</v>
@@ -1206,7 +1206,7 @@
         <v>270034912</v>
       </c>
       <c r="AF6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:32" x14ac:dyDescent="0.25">
@@ -1220,7 +1220,7 @@
         <v>269795</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E7" s="1">
         <v>576130</v>
@@ -1235,19 +1235,19 @@
         <v>2100955</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K7" s="1">
         <v>2609174</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N7" s="1">
         <v>2002690</v>
@@ -1259,40 +1259,40 @@
         <v>1294820</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W7" s="1">
         <v>1102637</v>
       </c>
       <c r="X7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z7" s="1">
         <v>1284993</v>
       </c>
       <c r="AA7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC7" s="1">
         <v>1378030</v>
@@ -1304,7 +1304,7 @@
         <v>2700089</v>
       </c>
       <c r="AF7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:32" x14ac:dyDescent="0.25">
@@ -1333,19 +1333,19 @@
         <v>33114492</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K8" s="1">
         <v>20150600</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N8" s="1">
         <v>26589864</v>
@@ -1357,19 +1357,19 @@
         <v>15688092</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V8" s="1">
         <v>14900795</v>
@@ -1378,19 +1378,19 @@
         <v>15456133</v>
       </c>
       <c r="X8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z8" s="1">
         <v>18790172</v>
       </c>
       <c r="AA8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC8" s="1">
         <v>22289092</v>
@@ -1402,7 +1402,7 @@
         <v>18420064</v>
       </c>
       <c r="AF8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.25">
@@ -1431,16 +1431,16 @@
         <v>23392484</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K9" s="1">
         <v>17730992</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M9" s="1">
         <v>35463040</v>
@@ -1455,40 +1455,40 @@
         <v>17402096</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W9" s="1">
         <v>9880658</v>
       </c>
       <c r="X9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z9" s="1">
         <v>11671525</v>
       </c>
       <c r="AA9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC9" s="1">
         <v>20356156</v>
@@ -1500,7 +1500,7 @@
         <v>16029204</v>
       </c>
       <c r="AF9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.25">
@@ -1514,7 +1514,7 @@
         <v>1134461</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="1">
         <v>6992049</v>
@@ -1523,25 +1523,25 @@
         <v>7700000</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H10" s="1">
         <v>8000000</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K10" s="1">
         <v>5200000</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N10" s="1">
         <v>7967589</v>
@@ -1553,19 +1553,19 @@
         <v>8000000</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V10" s="1">
         <v>4709819</v>
@@ -1574,19 +1574,19 @@
         <v>5090693</v>
       </c>
       <c r="X10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z10" s="1">
         <v>9080755</v>
       </c>
       <c r="AA10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC10" s="1">
         <v>4730882</v>
@@ -1598,7 +1598,7 @@
         <v>4984532</v>
       </c>
       <c r="AF10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:32" x14ac:dyDescent="0.25">
@@ -1627,19 +1627,19 @@
         <v>10458639</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K11" s="1">
         <v>13100000</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N11" s="1">
         <v>2607045</v>
@@ -1651,19 +1651,19 @@
         <v>5000000</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V11" s="1">
         <v>5113914</v>
@@ -1672,19 +1672,19 @@
         <v>6565038</v>
       </c>
       <c r="X11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z11" s="1">
         <v>11403714</v>
       </c>
       <c r="AA11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC11" s="1">
         <v>3598734</v>
@@ -1696,7 +1696,7 @@
         <v>5927228</v>
       </c>
       <c r="AF11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.25">
@@ -1710,7 +1710,7 @@
         <v>6708221</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="1">
         <v>8386902</v>
@@ -1725,16 +1725,16 @@
         <v>12500000</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K12" s="1">
         <v>17600000</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M12" s="1">
         <v>7527926</v>
@@ -1749,19 +1749,19 @@
         <v>7900000</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V12" s="1">
         <v>5301345</v>
@@ -1770,19 +1770,19 @@
         <v>2900000</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z12" s="1">
         <v>12335003</v>
       </c>
       <c r="AA12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC12" s="1">
         <v>7402867</v>
@@ -1794,7 +1794,7 @@
         <v>10704633</v>
       </c>
       <c r="AF12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:32" x14ac:dyDescent="0.25">
@@ -1808,7 +1808,7 @@
         <v>6993317</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E13" s="1">
         <v>5282649</v>
@@ -1823,16 +1823,16 @@
         <v>8953417</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K13" s="1">
         <v>10918762</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M13" s="1">
         <v>18816812</v>
@@ -1847,19 +1847,19 @@
         <v>8087311</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V13" s="1">
         <v>11229138</v>
@@ -1868,19 +1868,19 @@
         <v>5589951</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z13" s="1">
         <v>10157185</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC13" s="1">
         <v>11204850</v>
@@ -1892,7 +1892,7 @@
         <v>9849263</v>
       </c>
       <c r="AF13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:32" x14ac:dyDescent="0.25">
@@ -1921,19 +1921,19 @@
         <v>14655352</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K14" s="1">
         <v>10912028</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N14" s="1">
         <v>17817886</v>
@@ -1948,16 +1948,16 @@
         <v>72822120</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V14" s="1">
         <v>5468311</v>
@@ -1966,22 +1966,22 @@
         <v>6209861</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z14" s="1">
         <v>25390872</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD14" s="1">
         <v>10116575</v>
@@ -1990,7 +1990,7 @@
         <v>19121916</v>
       </c>
       <c r="AF14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.25">
@@ -2004,7 +2004,7 @@
         <v>16554</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E15" s="1">
         <v>59927</v>
@@ -2019,16 +2019,16 @@
         <v>232561</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K15" s="1">
         <v>210002</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M15" s="1">
         <v>53732</v>
@@ -2043,40 +2043,40 @@
         <v>178335</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W15" s="1">
         <v>131841</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z15" s="1">
         <v>149194</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC15" s="1">
         <v>125489</v>
@@ -2088,7 +2088,7 @@
         <v>344002</v>
       </c>
       <c r="AF15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.25">
@@ -2117,16 +2117,16 @@
         <v>28322788</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K16" s="1">
         <v>31757462</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M16" s="1">
         <v>31845456</v>
@@ -2141,19 +2141,19 @@
         <v>13587076</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V16" s="1">
         <v>17067468</v>
@@ -2162,19 +2162,19 @@
         <v>14353922</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z16" s="1">
         <v>27070660</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC16" s="1">
         <v>23857540</v>
@@ -2186,7 +2186,7 @@
         <v>24390084</v>
       </c>
       <c r="AF16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.25">
@@ -2215,19 +2215,19 @@
         <v>9975474</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K17" s="1">
         <v>5517771</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N17" s="1">
         <v>5683286</v>
@@ -2239,19 +2239,19 @@
         <v>3614533</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V17" s="1">
         <v>1704234</v>
@@ -2260,19 +2260,19 @@
         <v>3277740</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z17" s="1">
         <v>4042454</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC17" s="1">
         <v>3157881</v>
@@ -2284,7 +2284,7 @@
         <v>5638650</v>
       </c>
       <c r="AF17" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
@@ -2298,7 +2298,7 @@
         <v>1221853</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E18" s="1">
         <v>1836158</v>
@@ -2307,22 +2307,22 @@
         <v>1883141</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H18" s="1">
         <v>5026086</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M18" s="1">
         <v>4524402</v>
@@ -2340,37 +2340,37 @@
         <v>243390</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W18" s="1">
         <v>2252149</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z18" s="1">
         <v>2692015</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC18" s="1">
         <v>2825136</v>
@@ -2382,7 +2382,7 @@
         <v>2244363</v>
       </c>
       <c r="AF18" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:32" x14ac:dyDescent="0.25">
@@ -2411,16 +2411,16 @@
         <v>9300000</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K19" s="1">
         <v>9400000</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M19" s="1">
         <v>5309012</v>
@@ -2435,40 +2435,40 @@
         <v>6200000</v>
       </c>
       <c r="Q19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V19" s="1">
         <v>7413925</v>
       </c>
       <c r="W19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z19" s="1">
         <v>7523563</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC19" s="1">
         <v>7954070</v>
@@ -2480,7 +2480,7 @@
         <v>4458893</v>
       </c>
       <c r="AF19" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:32" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
         <v>387461</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E20" s="1">
         <v>1300023</v>
@@ -2509,19 +2509,19 @@
         <v>3601530</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K20" s="1">
         <v>3480255</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N20" s="1">
         <v>3694972</v>
@@ -2536,37 +2536,37 @@
         <v>642913</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W20" s="1">
         <v>2277603</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z20" s="1">
         <v>2692532</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC20" s="1">
         <v>3147605</v>
@@ -2578,7 +2578,7 @@
         <v>2891937</v>
       </c>
       <c r="AF20" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:32" x14ac:dyDescent="0.25">
@@ -2607,16 +2607,16 @@
         <v>1967802</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K21" s="1">
         <v>1494687</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M21" s="1">
         <v>2173057</v>
@@ -2631,19 +2631,19 @@
         <v>953409</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V21" s="1">
         <v>575105</v>
@@ -2652,19 +2652,19 @@
         <v>1129530</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z21" s="1">
         <v>1510539</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC21" s="1">
         <v>1396205</v>
@@ -2676,12 +2676,12 @@
         <v>1960914</v>
       </c>
       <c r="AF21" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1">
         <v>8136393</v>
@@ -2705,19 +2705,19 @@
         <v>19265532</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K22" s="1">
         <v>19751814</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N22" s="1">
         <v>26002884</v>
@@ -2729,40 +2729,40 @@
         <v>22318676</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="V22" s="5">
+        <v>44220462</v>
       </c>
       <c r="W22" s="1">
         <v>16863836</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z22" s="1">
         <v>16341826</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC22" s="1">
         <v>35732140</v>
@@ -2774,12 +2774,12 @@
         <v>32319858</v>
       </c>
       <c r="AF22" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="1">
         <v>330358</v>
@@ -2788,7 +2788,7 @@
         <v>41068</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E23" s="1">
         <v>121879</v>
@@ -2803,19 +2803,19 @@
         <v>689932</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K23" s="1">
         <v>825668</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="N23" s="1">
         <v>752806</v>
@@ -2827,40 +2827,40 @@
         <v>389357</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W23" s="1">
         <v>368810</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z23" s="1">
         <v>340138</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC23" s="1">
         <v>493999</v>
@@ -2872,12 +2872,12 @@
         <v>869652</v>
       </c>
       <c r="AF23" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="1">
         <v>15500000</v>
@@ -2886,7 +2886,7 @@
         <v>21581340</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E24" s="1">
         <v>21126699</v>
@@ -2901,10 +2901,10 @@
         <v>42859368</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K24" s="1">
         <v>43318484</v>
@@ -2925,19 +2925,19 @@
         <v>42360027</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V24" s="1">
         <v>19553284</v>
@@ -2946,19 +2946,19 @@
         <v>16344265</v>
       </c>
       <c r="X24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z24" s="1">
         <v>51515808</v>
       </c>
       <c r="AA24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC24" s="1">
         <v>21114584</v>
@@ -2970,12 +2970,12 @@
         <v>30150764</v>
       </c>
       <c r="AF24" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="25" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="1">
         <v>8603850</v>
@@ -2999,7 +2999,7 @@
         <v>9716813</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J25" s="1">
         <v>7763694</v>
@@ -3008,7 +3008,7 @@
         <v>11801656</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M25" s="1">
         <v>15394652</v>
@@ -3023,19 +3023,19 @@
         <v>6975576</v>
       </c>
       <c r="Q25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V25" s="1">
         <v>4990454</v>
@@ -3044,19 +3044,19 @@
         <v>7646855</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z25" s="1">
         <v>11950872</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC25" s="1">
         <v>8846122</v>
@@ -3068,12 +3068,12 @@
         <v>10852976</v>
       </c>
       <c r="AF25" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="1">
         <v>11000000</v>
@@ -3082,7 +3082,7 @@
         <v>4682113</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E26" s="1">
         <v>10930219</v>
@@ -3097,16 +3097,16 @@
         <v>12778780</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K26" s="1">
         <v>10500000</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M26" s="1">
         <v>12319913</v>
@@ -3121,19 +3121,19 @@
         <v>9300000</v>
       </c>
       <c r="Q26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V26" s="1">
         <v>8303368</v>
@@ -3142,19 +3142,19 @@
         <v>7042850</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z26" s="1">
         <v>9657745</v>
       </c>
       <c r="AA26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC26" s="1">
         <v>10389487</v>
@@ -3166,12 +3166,12 @@
         <v>9007044</v>
       </c>
       <c r="AF26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="1">
         <v>1747244</v>
@@ -3195,16 +3195,16 @@
         <v>2593586</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K27" s="1">
         <v>3154225</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M27" s="1">
         <v>4713140</v>
@@ -3219,40 +3219,40 @@
         <v>3202816</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="W27" s="1">
         <v>3359220</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z27" s="1">
         <v>2556451</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC27" s="1">
         <v>3717816</v>
@@ -3264,12 +3264,12 @@
         <v>2554355</v>
       </c>
       <c r="AF27" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="1">
         <v>30018598</v>
@@ -3293,16 +3293,16 @@
         <v>70631008</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="K28" s="1">
         <v>42344279</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="M28" s="1">
         <v>90721728</v>
@@ -3317,19 +3317,19 @@
         <v>28547412</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="V28" s="1">
         <v>21215104</v>
@@ -3338,19 +3338,19 @@
         <v>29643627</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Z28" s="1">
         <v>39582696</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AC28" s="1">
         <v>31788260</v>
@@ -3362,12 +3362,12 @@
         <v>26338052</v>
       </c>
       <c r="AF28" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="1">
         <v>86446111</v>
@@ -3465,7 +3465,7 @@
     </row>
     <row r="30" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="1">
         <v>412563408</v>

</xml_diff>

<commit_message>
Updated Box Office by Country, Google Maps, Images
</commit_message>
<xml_diff>
--- a/Datasets/Box_Office_by_Country.xlsx
+++ b/Datasets/Box_Office_by_Country.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee Wealth Mgmt\Documents\GitHub\Team-Aurora-Marvels\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53468562-86DD-4367-812A-6A0A04FFD248}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1078E96E-0465-42A7-904D-9E4AE964CB9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" xr2:uid="{52C63866-7CA8-46D1-AE34-6D66B8611C4C}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="63">
   <si>
     <t>Country</t>
   </si>
@@ -595,9 +595,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5B63F0-7E42-422D-B61C-0353DBECD408}">
   <dimension ref="A1:AF33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="V22" sqref="V22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -884,8 +882,8 @@
       <c r="S3" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="V3" s="1" t="s">
-        <v>61</v>
+      <c r="V3" s="1">
+        <v>36164486</v>
       </c>
       <c r="W3" s="1">
         <v>17295477</v>

</xml_diff>

<commit_message>
Minor changes to Box Office by Country
</commit_message>
<xml_diff>
--- a/Datasets/Box_Office_by_Country.xlsx
+++ b/Datasets/Box_Office_by_Country.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee Wealth Mgmt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lee Wealth Mgmt\Documents\GitHub\Team-Aurora-Marvels\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{808D15AE-7FF7-44DF-A81E-88C70B3ECCB7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B703237A-F00D-4158-AAAE-CA863E60F6A5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7665" xr2:uid="{52C63866-7CA8-46D1-AE34-6D66B8611C4C}"/>
   </bookViews>
@@ -222,9 +222,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
-  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -261,7 +258,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -272,10 +269,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,12 +583,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF5B63F0-7E42-422D-B61C-0353DBECD408}">
-  <dimension ref="A1:AF32"/>
+  <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3568,44 +3558,6 @@
         <v>374825760</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-    </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="6"/>
-      <c r="I32" s="6"/>
-      <c r="J32" s="6"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
-      <c r="N32" s="6"/>
-      <c r="O32" s="6"/>
-      <c r="P32" s="6"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
-      <c r="S32" s="6"/>
-      <c r="T32" s="6"/>
-      <c r="U32" s="6"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="6"/>
-      <c r="X32" s="6"/>
-      <c r="Y32" s="6"/>
-      <c r="Z32" s="6"/>
-      <c r="AA32" s="6"/>
-      <c r="AB32" s="6"/>
-      <c r="AC32" s="6"/>
-      <c r="AD32" s="6"/>
-      <c r="AE32" s="6"/>
-      <c r="AF32" s="6"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>